<commit_message>
Extensión del periodo temporal de la base
</commit_message>
<xml_diff>
--- a/data/otras/trade.xlsx
+++ b/data/otras/trade.xlsx
@@ -5,17 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diplomado CSC\Proyecto China\otros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diplomado CSC\proyecto-china\data\otras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13407F4C-2E6F-42B7-8B34-E6738C995E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9923C163-0749-4D77-91C8-9C85DF3EDA11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -952,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2258" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2272" sqref="A2272"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>